<commit_message>
NOT IMPORTANT (new data results)
</commit_message>
<xml_diff>
--- a/tracks_vs_colors.xlsx
+++ b/tracks_vs_colors.xlsx
@@ -457,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,19 +499,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
@@ -521,19 +521,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
@@ -543,19 +543,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -565,19 +565,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
@@ -666,28 +666,6 @@
       </c>
       <c r="F9" t="n">
         <v>20</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>0000</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>15</v>
-      </c>
-      <c r="C10" t="n">
-        <v>15</v>
-      </c>
-      <c r="D10" t="n">
-        <v>15</v>
-      </c>
-      <c r="E10" t="n">
-        <v>15</v>
-      </c>
-      <c r="F10" t="n">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>